<commit_message>
action_type queries and last arketip sqls added
</commit_message>
<xml_diff>
--- a/Digital Data for arketypes_reviewed version_OK.xlsx
+++ b/Digital Data for arketypes_reviewed version_OK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kerembukucu/Desktop/airflow-docker-project/dags/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A090C3AA-CBBF-004A-AC52-F9A9D92D4E63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38D9B3FD-C50E-4148-B314-466626FA678A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main sheet" sheetId="5" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="286">
   <si>
     <t>profilingScore</t>
   </si>
@@ -965,12 +965,6 @@
     <t>Kerem</t>
   </si>
   <si>
-    <t>portfoy ekrani acip fonu sattigini tesbit edebiliriz ama fonun zararda oldugu icin mi sattigini nasil anlayacagiz, fonlarin degerlerinin zaman icinde degisiminin bilgisine ihtiyac var</t>
-  </si>
-  <si>
-    <t>populer fonlar bilgisine ihtiyac var</t>
-  </si>
-  <si>
     <t>digital_actions, view_name kolonu feeds, details kolonu close olanlar sayildi, saat 22 ile 6 arasindaki 8 saatlik dilimdekiler gece olarak sayildi</t>
   </si>
   <si>
@@ -984,6 +978,46 @@
   </si>
   <si>
     <t xml:space="preserve">musterinin actions tablosunda open yaptigi fonlar arasinda katilim fonlarinin orani yuzde 80'den fazla ise bu kolon 1 </t>
+  </si>
+  <si>
+    <t>IGNORED</t>
+  </si>
+  <si>
+    <t>musteri o fonu aldiginda, populer fon olup olmadigi kontrole edilecek</t>
+  </si>
+  <si>
+    <t>portfoy ekrani acip fonu sattigini tesbit edebiliriz ama fonun zararda oldugu icin mi sattigini nasil anlayacagiz, fonlarin degerlerinin zaman icinde degisiminin bilgisine ihtiyac var…. Step 2</t>
+  </si>
+  <si>
+    <t>actions tablosuna gelecek</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>video_izleyen</t>
+  </si>
+  <si>
+    <t>dya_gece</t>
+  </si>
+  <si>
+    <t>actions tablosunu gözlemler. Her bir customer_id için, action_type sütunu 'Fon Alma' ise, fund_code sütunundaki fon kodunu alır, bu fonun popüler fonlar arasında olup olmadığını, az önce oluşturduğumuz tabloya (popular_funds) bakarak kontrol eder. Sonuç olarak, müşterinin popüler fon aldığı işlem sayısının, toplam fon aldığı işlem sayısına oranını (0 ile 1 arasında bir float sayı) döndürür. Denklem:
+popüler fon alım sayısı / toplam fon alım sayısı</t>
+  </si>
+  <si>
+    <t>popular_fund_ratio</t>
+  </si>
+  <si>
+    <t>dws.actions tablosunda actiion_type kolonunda 'Yeni Portföy Oluşturma' olan musteriler 1 digerleri 0 olarak sayildi</t>
+  </si>
+  <si>
+    <t>yeni_portfoy</t>
+  </si>
+  <si>
+    <t>dws.actions tablosunda actiion_type kolonunda 'Birden Fazla Banka Hesabı Var mı?'olan musteriler 1 digerleri 0 olarak sayildi</t>
+  </si>
+  <si>
+    <t>birden_fazla_banka_hesabi</t>
   </si>
 </sst>
 </file>
@@ -1222,7 +1256,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1291,9 +1325,6 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1321,51 +1352,123 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{EFAE8721-CC24-C549-AC8F-5A9B7A4142B7}"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="25">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="8"/>
+        <family val="2"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1600,13 +1703,6 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
@@ -1633,6 +1729,13 @@
         <family val="2"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1669,69 +1772,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -1746,42 +1786,43 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F6E77058-CC74-E949-A562-E78F1A066BCA}" name="Table3" displayName="Table3" ref="A1:H33" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" headerRowBorderDxfId="9" tableBorderDxfId="10" totalsRowBorderDxfId="8">
-  <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{0DC4A6E6-C276-CD4E-A928-CCF79291A43F}" name="TİP" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{9A26924A-2D71-C541-9E27-CE86E426C6C0}" name="Özellik" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{8D496CF0-8DD5-7243-81EA-7FFB647FA4D5}" name="View Name - Details" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{77DF62AD-D442-5C44-8268-07B68C6FE7F5}" name="VERI NASIL URETILDI" dataDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{788555F5-3C2E-5248-A587-1959FAB6B71E}" name="ilgili kolonun adi" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{9BCC0744-1262-45DD-94F3-1743C1BED361}" name="teknik notlar" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{7D22B9A8-4388-45CA-B94F-5E7970B2BFF9}" name="Ozgur Yorum" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{F784A7B7-1F96-6B45-AE3B-B51E35F10C92}" name="Kerem" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F6E77058-CC74-E949-A562-E78F1A066BCA}" name="Table3" displayName="Table3" ref="A1:I33" totalsRowShown="0" headerRowDxfId="24" dataDxfId="22" headerRowBorderDxfId="23" tableBorderDxfId="21" totalsRowBorderDxfId="20">
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{0DC4A6E6-C276-CD4E-A928-CCF79291A43F}" name="TİP" dataDxfId="19"/>
+    <tableColumn id="2" xr3:uid="{9A26924A-2D71-C541-9E27-CE86E426C6C0}" name="Özellik" dataDxfId="18"/>
+    <tableColumn id="4" xr3:uid="{8D496CF0-8DD5-7243-81EA-7FFB647FA4D5}" name="View Name - Details" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{77DF62AD-D442-5C44-8268-07B68C6FE7F5}" name="VERI NASIL URETILDI" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{788555F5-3C2E-5248-A587-1959FAB6B71E}" name="ilgili kolonun adi" dataDxfId="15"/>
+    <tableColumn id="7" xr3:uid="{9BCC0744-1262-45DD-94F3-1743C1BED361}" name="teknik notlar" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{7D22B9A8-4388-45CA-B94F-5E7970B2BFF9}" name="Ozgur Yorum" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{F784A7B7-1F96-6B45-AE3B-B51E35F10C92}" name="Kerem" dataDxfId="12"/>
+    <tableColumn id="8" xr3:uid="{F668BCD7-6BBC-3E41-BCC3-3256AB9346AA}" name="Column1" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CB319A93-8689-B84B-9660-5C70A8095955}" name="Table2" displayName="Table2" ref="A1:G7" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{CB319A93-8689-B84B-9660-5C70A8095955}" name="Table2" displayName="Table2" ref="A1:G7" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="A1:G7" xr:uid="{CB319A93-8689-B84B-9660-5C70A8095955}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{02A22B36-9860-AE42-831E-45383F966ECE}" name="FONERIALI" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{0214F33B-5915-B84F-AAC7-109FF9E03E69}" name="ARAŞTIRMACI" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{BEB36767-0B1C-F14E-BB11-F2F3E2145A19}" name="KATILIM" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{AD89E59B-7A8C-CD4A-B465-9B781E246812}" name="DETAYCI" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{FF915929-8EB1-9A41-A565-8A4056C174DF}" name="NEWBIE" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{B1E6AA5B-0BC9-DA4B-B466-470B58DE298E}" name="GECE KUŞU" dataDxfId="16"/>
-    <tableColumn id="7" xr3:uid="{F55D0A82-475B-A644-BC0E-B356BE807DC8}" name="AİLE İNSANI" dataDxfId="15"/>
+    <tableColumn id="1" xr3:uid="{02A22B36-9860-AE42-831E-45383F966ECE}" name="FONERIALI" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{0214F33B-5915-B84F-AAC7-109FF9E03E69}" name="ARAŞTIRMACI" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{BEB36767-0B1C-F14E-BB11-F2F3E2145A19}" name="KATILIM" dataDxfId="7"/>
+    <tableColumn id="4" xr3:uid="{AD89E59B-7A8C-CD4A-B465-9B781E246812}" name="DETAYCI" dataDxfId="6"/>
+    <tableColumn id="5" xr3:uid="{FF915929-8EB1-9A41-A565-8A4056C174DF}" name="NEWBIE" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{B1E6AA5B-0BC9-DA4B-B466-470B58DE298E}" name="GECE KUŞU" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{F55D0A82-475B-A644-BC0E-B356BE807DC8}" name="AİLE İNSANI" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D1FB2435-7CEE-4A43-839B-EC14451A3106}" name="Table1" displayName="Table1" ref="A3:G10" totalsRowShown="0" headerRowDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D1FB2435-7CEE-4A43-839B-EC14451A3106}" name="Table1" displayName="Table1" ref="A3:G10" totalsRowShown="0" headerRowDxfId="2">
   <autoFilter ref="A3:G10" xr:uid="{D1FB2435-7CEE-4A43-839B-EC14451A3106}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{E5D08E52-3AAA-E644-8D43-C1A6AB96E18C}" name="Kullanıcı Tipi" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{E5D08E52-3AAA-E644-8D43-C1A6AB96E18C}" name="Kullanıcı Tipi" dataDxfId="1"/>
     <tableColumn id="2" xr3:uid="{2549D7FF-9F22-824E-B993-B31225B38DDF}" name="Açıklama 1"/>
     <tableColumn id="3" xr3:uid="{FB5ED99B-14B9-D446-B253-9BD9DB0C6DC0}" name="Açıklama 2"/>
     <tableColumn id="4" xr3:uid="{E4A1315C-B804-F74A-BA33-38999FD8CC9C}" name="Açıklama 3"/>
@@ -2080,10 +2121,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0C6CCB9-9732-704F-BE94-AFE20FC898AB}">
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="125" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32:H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.5" defaultRowHeight="11"/>
@@ -2093,12 +2134,12 @@
     <col min="3" max="3" width="14.83203125" style="4" customWidth="1"/>
     <col min="4" max="4" width="35.5" style="4" customWidth="1"/>
     <col min="5" max="5" width="14.83203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="55" style="25" customWidth="1"/>
-    <col min="7" max="8" width="32.6640625" style="25" customWidth="1"/>
+    <col min="6" max="6" width="55" style="24" customWidth="1"/>
+    <col min="7" max="8" width="32.6640625" style="24" customWidth="1"/>
     <col min="9" max="16384" width="7.5" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="12">
+    <row r="1" spans="1:9" ht="12">
       <c r="A1" s="6" t="s">
         <v>165</v>
       </c>
@@ -2114,17 +2155,20 @@
       <c r="E1" s="7" t="s">
         <v>229</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="32" t="s">
         <v>248</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="32" t="s">
         <v>249</v>
       </c>
-      <c r="H1" s="34" t="s">
+      <c r="H1" s="33" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" ht="60">
+      <c r="I1" s="42" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="60">
       <c r="A2" s="8" t="s">
         <v>3</v>
       </c>
@@ -2146,9 +2190,9 @@
       <c r="G2" s="16" t="s">
         <v>250</v>
       </c>
-      <c r="H2" s="37"/>
-    </row>
-    <row r="3" spans="1:8" ht="36">
+      <c r="H2" s="35"/>
+    </row>
+    <row r="3" spans="1:9" ht="36">
       <c r="A3" s="8" t="s">
         <v>3</v>
       </c>
@@ -2166,9 +2210,9 @@
         <v>199</v>
       </c>
       <c r="G3" s="16"/>
-      <c r="H3" s="37"/>
-    </row>
-    <row r="4" spans="1:8" ht="108">
+      <c r="H3" s="35"/>
+    </row>
+    <row r="4" spans="1:9" ht="108">
       <c r="A4" s="8" t="s">
         <v>3</v>
       </c>
@@ -2188,9 +2232,9 @@
         <v>196</v>
       </c>
       <c r="G4" s="16"/>
-      <c r="H4" s="37"/>
-    </row>
-    <row r="5" spans="1:8" ht="36">
+      <c r="H4" s="35"/>
+    </row>
+    <row r="5" spans="1:9" ht="36">
       <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
@@ -2206,15 +2250,15 @@
       <c r="E5" s="5" t="s">
         <v>261</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="34" t="s">
         <v>189</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="34" t="s">
         <v>251</v>
       </c>
-      <c r="H5" s="38"/>
-    </row>
-    <row r="6" spans="1:8" ht="60">
+      <c r="H5" s="36"/>
+    </row>
+    <row r="6" spans="1:9" ht="60">
       <c r="A6" s="8" t="s">
         <v>3</v>
       </c>
@@ -2232,9 +2276,9 @@
         <v>200</v>
       </c>
       <c r="G6" s="23"/>
-      <c r="H6" s="39"/>
-    </row>
-    <row r="7" spans="1:8" ht="12">
+      <c r="H6" s="37"/>
+    </row>
+    <row r="7" spans="1:9" ht="12">
       <c r="A7" s="8" t="s">
         <v>3</v>
       </c>
@@ -2254,9 +2298,9 @@
         <v>194</v>
       </c>
       <c r="G7" s="16"/>
-      <c r="H7" s="37"/>
-    </row>
-    <row r="8" spans="1:8" ht="120">
+      <c r="H7" s="35"/>
+    </row>
+    <row r="8" spans="1:9" ht="120">
       <c r="A8" s="13" t="s">
         <v>4</v>
       </c>
@@ -2274,16 +2318,16 @@
         <v>201</v>
       </c>
       <c r="G8" s="22"/>
-      <c r="H8" s="40"/>
-    </row>
-    <row r="9" spans="1:8" ht="12">
+      <c r="H8" s="38"/>
+    </row>
+    <row r="9" spans="1:9" ht="12">
       <c r="A9" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="26" t="s">
         <v>139</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="26" t="s">
         <v>168</v>
       </c>
       <c r="D9" s="12" t="s">
@@ -2296,16 +2340,16 @@
         <v>194</v>
       </c>
       <c r="G9" s="16"/>
-      <c r="H9" s="37"/>
-    </row>
-    <row r="10" spans="1:8" ht="24">
+      <c r="H9" s="35"/>
+    </row>
+    <row r="10" spans="1:9" ht="24">
       <c r="A10" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="26" t="s">
         <v>169</v>
       </c>
       <c r="D10" s="12" t="s">
@@ -2318,16 +2362,16 @@
         <v>194</v>
       </c>
       <c r="G10" s="16"/>
-      <c r="H10" s="37"/>
-    </row>
-    <row r="11" spans="1:8" ht="72">
+      <c r="H10" s="35"/>
+    </row>
+    <row r="11" spans="1:9" ht="72">
       <c r="A11" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="C11" s="27"/>
+      <c r="C11" s="26"/>
       <c r="D11" s="12" t="s">
         <v>216</v>
       </c>
@@ -2338,9 +2382,9 @@
         <v>202</v>
       </c>
       <c r="G11" s="22"/>
-      <c r="H11" s="40"/>
-    </row>
-    <row r="12" spans="1:8" ht="24">
+      <c r="H11" s="38"/>
+    </row>
+    <row r="12" spans="1:9" ht="24">
       <c r="A12" s="14" t="s">
         <v>4</v>
       </c>
@@ -2358,23 +2402,25 @@
       <c r="G12" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="H12" s="41"/>
-    </row>
-    <row r="13" spans="1:8" ht="132">
+      <c r="H12" s="39" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="132">
       <c r="A13" s="15" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="26" t="s">
         <v>171</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="F13" s="22" t="s">
         <v>203</v>
@@ -2382,16 +2428,16 @@
       <c r="G13" s="22" t="s">
         <v>252</v>
       </c>
-      <c r="H13" s="40"/>
-    </row>
-    <row r="14" spans="1:8" ht="144">
+      <c r="H13" s="38"/>
+    </row>
+    <row r="14" spans="1:9" ht="144">
       <c r="A14" s="15" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="C14" s="27"/>
+      <c r="C14" s="26"/>
       <c r="D14" s="12" t="s">
         <v>263</v>
       </c>
@@ -2404,16 +2450,16 @@
       <c r="G14" s="16" t="s">
         <v>254</v>
       </c>
-      <c r="H14" s="37"/>
-    </row>
-    <row r="15" spans="1:8" ht="24">
+      <c r="H14" s="35"/>
+    </row>
+    <row r="15" spans="1:9" ht="24">
       <c r="A15" s="15" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="C15" s="27"/>
+      <c r="C15" s="26"/>
       <c r="D15" s="12" t="s">
         <v>265</v>
       </c>
@@ -2426,16 +2472,16 @@
       <c r="G15" s="16" t="s">
         <v>253</v>
       </c>
-      <c r="H15" s="37"/>
-    </row>
-    <row r="16" spans="1:8" ht="24">
+      <c r="H15" s="35"/>
+    </row>
+    <row r="16" spans="1:9" ht="24">
       <c r="A16" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="26" t="s">
         <v>146</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="26" t="s">
         <v>2</v>
       </c>
       <c r="D16" s="12" t="s">
@@ -2448,16 +2494,16 @@
         <v>191</v>
       </c>
       <c r="G16" s="16"/>
-      <c r="H16" s="37"/>
-    </row>
-    <row r="17" spans="1:8" ht="12">
+      <c r="H16" s="35"/>
+    </row>
+    <row r="17" spans="1:9" ht="12">
       <c r="A17" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="26" t="s">
         <v>147</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="26" t="s">
         <v>173</v>
       </c>
       <c r="D17" s="12" t="s">
@@ -2468,16 +2514,16 @@
         <v>193</v>
       </c>
       <c r="G17" s="16"/>
-      <c r="H17" s="37"/>
-    </row>
-    <row r="18" spans="1:8" ht="12">
+      <c r="H17" s="35"/>
+    </row>
+    <row r="18" spans="1:9" ht="12">
       <c r="A18" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="26" t="s">
         <v>174</v>
       </c>
       <c r="D18" s="12" t="s">
@@ -2490,16 +2536,16 @@
         <v>192</v>
       </c>
       <c r="G18" s="16"/>
-      <c r="H18" s="37"/>
-    </row>
-    <row r="19" spans="1:8" ht="24">
+      <c r="H18" s="35"/>
+    </row>
+    <row r="19" spans="1:9" ht="24">
       <c r="A19" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="26" t="s">
         <v>149</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="27" t="s">
         <v>175</v>
       </c>
       <c r="D19" s="12" t="s">
@@ -2512,31 +2558,31 @@
         <v>194</v>
       </c>
       <c r="G19" s="16"/>
-      <c r="H19" s="37"/>
-    </row>
-    <row r="20" spans="1:8" ht="24">
+      <c r="H19" s="35"/>
+    </row>
+    <row r="20" spans="1:9" ht="24">
       <c r="A20" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="26" t="s">
         <v>150</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="27" t="s">
         <v>176</v>
       </c>
-      <c r="D20" s="29" t="s">
+      <c r="D20" s="28" t="s">
         <v>220</v>
       </c>
-      <c r="E20" s="29" t="s">
+      <c r="E20" s="28" t="s">
         <v>240</v>
       </c>
       <c r="F20" s="16" t="s">
         <v>194</v>
       </c>
       <c r="G20" s="16"/>
-      <c r="H20" s="37"/>
-    </row>
-    <row r="21" spans="1:8" ht="132">
+      <c r="H20" s="35"/>
+    </row>
+    <row r="21" spans="1:9" ht="132">
       <c r="A21" s="18" t="s">
         <v>7</v>
       </c>
@@ -2546,288 +2592,308 @@
       <c r="C21" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="D21" s="20"/>
+      <c r="D21" s="20" t="s">
+        <v>280</v>
+      </c>
       <c r="E21" s="20"/>
-      <c r="F21" s="44" t="s">
+      <c r="F21" s="40" t="s">
         <v>206</v>
       </c>
-      <c r="G21" s="44" t="s">
+      <c r="G21" s="40" t="s">
         <v>255</v>
       </c>
-      <c r="H21" s="45" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" ht="60">
+      <c r="H21" s="41" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="108">
       <c r="A22" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="26" t="s">
         <v>152</v>
       </c>
-      <c r="C22" s="19" t="s">
+      <c r="C22" s="27" t="s">
         <v>178</v>
       </c>
-      <c r="D22" s="20"/>
-      <c r="E22" s="20"/>
-      <c r="F22" s="44" t="s">
+      <c r="D22" s="28" t="s">
+        <v>280</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>281</v>
+      </c>
+      <c r="F22" s="16" t="s">
         <v>207</v>
       </c>
-      <c r="G22" s="44" t="s">
+      <c r="G22" s="16" t="s">
         <v>256</v>
       </c>
-      <c r="H22" s="46" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" ht="24">
+      <c r="H22" s="35" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="24">
       <c r="A23" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="26" t="s">
         <v>153</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="27" t="s">
         <v>179</v>
       </c>
-      <c r="D23" s="29" t="s">
+      <c r="D23" s="28" t="s">
         <v>221</v>
       </c>
-      <c r="E23" s="29" t="s">
+      <c r="E23" s="28" t="s">
         <v>241</v>
       </c>
       <c r="F23" s="16" t="s">
         <v>194</v>
       </c>
       <c r="G23" s="16"/>
-      <c r="H23" s="37"/>
-    </row>
-    <row r="24" spans="1:8" ht="24">
+      <c r="H23" s="35"/>
+    </row>
+    <row r="24" spans="1:9" ht="24">
       <c r="A24" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="C24" s="28" t="s">
+      <c r="C24" s="27" t="s">
         <v>180</v>
       </c>
-      <c r="D24" s="29" t="s">
+      <c r="D24" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="E24" s="29" t="s">
+      <c r="E24" s="28" t="s">
         <v>242</v>
       </c>
       <c r="F24" s="16" t="s">
         <v>194</v>
       </c>
       <c r="G24" s="16"/>
-      <c r="H24" s="37"/>
-    </row>
-    <row r="25" spans="1:8" ht="36">
+      <c r="H24" s="35"/>
+    </row>
+    <row r="25" spans="1:9" ht="36">
       <c r="A25" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="26" t="s">
         <v>155</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="27" t="s">
         <v>195</v>
       </c>
-      <c r="D25" s="29" t="s">
+      <c r="D25" s="28" t="s">
         <v>223</v>
       </c>
-      <c r="E25" s="29" t="s">
+      <c r="E25" s="28" t="s">
         <v>243</v>
       </c>
       <c r="F25" s="16" t="s">
         <v>194</v>
       </c>
       <c r="G25" s="16"/>
-      <c r="H25" s="37"/>
-    </row>
-    <row r="26" spans="1:8" ht="36">
+      <c r="H25" s="35"/>
+    </row>
+    <row r="26" spans="1:9" ht="36">
       <c r="A26" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="27" t="s">
         <v>181</v>
       </c>
-      <c r="D26" s="29" t="s">
+      <c r="D26" s="28" t="s">
         <v>224</v>
       </c>
-      <c r="E26" s="29" t="s">
+      <c r="E26" s="28" t="s">
         <v>244</v>
       </c>
       <c r="F26" s="16" t="s">
         <v>194</v>
       </c>
       <c r="G26" s="16"/>
-      <c r="H26" s="37"/>
-    </row>
-    <row r="27" spans="1:8" ht="36">
+      <c r="H26" s="35"/>
+    </row>
+    <row r="27" spans="1:9" ht="36">
       <c r="A27" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="27" t="s">
+      <c r="B27" s="26" t="s">
         <v>157</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="27" t="s">
         <v>182</v>
       </c>
-      <c r="D27" s="29" t="s">
+      <c r="D27" s="28" t="s">
         <v>225</v>
       </c>
-      <c r="E27" s="29" t="s">
+      <c r="E27" s="28" t="s">
         <v>245</v>
       </c>
       <c r="F27" s="16" t="s">
         <v>194</v>
       </c>
       <c r="G27" s="16"/>
-      <c r="H27" s="37"/>
-    </row>
-    <row r="28" spans="1:8" ht="36">
+      <c r="H27" s="35"/>
+    </row>
+    <row r="28" spans="1:9" ht="36">
       <c r="A28" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="26" t="s">
         <v>158</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="27" t="s">
         <v>183</v>
       </c>
-      <c r="D28" s="29" t="s">
+      <c r="D28" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="E28" s="29" t="s">
+      <c r="E28" s="28" t="s">
         <v>246</v>
       </c>
       <c r="F28" s="16" t="s">
         <v>194</v>
       </c>
       <c r="G28" s="16"/>
-      <c r="H28" s="37"/>
-    </row>
-    <row r="29" spans="1:8" ht="36">
+      <c r="H28" s="35"/>
+    </row>
+    <row r="29" spans="1:9" ht="36">
       <c r="A29" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="26" t="s">
         <v>159</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="27" t="s">
         <v>184</v>
       </c>
-      <c r="D29" s="29" t="s">
-        <v>270</v>
-      </c>
-      <c r="E29" s="29"/>
+      <c r="D29" s="28" t="s">
+        <v>268</v>
+      </c>
+      <c r="E29" s="28" t="s">
+        <v>278</v>
+      </c>
       <c r="F29" s="16" t="s">
         <v>194</v>
       </c>
       <c r="G29" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="H29" s="37"/>
-    </row>
-    <row r="30" spans="1:8" ht="36">
+      <c r="H29" s="35"/>
+    </row>
+    <row r="30" spans="1:9" ht="36">
       <c r="A30" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="26" t="s">
         <v>160</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="27" t="s">
         <v>185</v>
       </c>
-      <c r="D30" s="29" t="s">
-        <v>271</v>
-      </c>
-      <c r="E30" s="29"/>
+      <c r="D30" s="28" t="s">
+        <v>269</v>
+      </c>
+      <c r="E30" s="28" t="s">
+        <v>279</v>
+      </c>
       <c r="F30" s="16" t="s">
         <v>194</v>
       </c>
       <c r="G30" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="H30" s="37"/>
-    </row>
-    <row r="31" spans="1:8" ht="24">
+      <c r="H30" s="35"/>
+    </row>
+    <row r="31" spans="1:9" ht="24">
       <c r="A31" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B31" s="11" t="s">
+      <c r="B31" s="26" t="s">
         <v>161</v>
       </c>
-      <c r="C31" s="19" t="s">
+      <c r="C31" s="27" t="s">
         <v>186</v>
       </c>
-      <c r="D31" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="E31" s="20"/>
-      <c r="F31" s="24" t="s">
+      <c r="D31" s="28" t="s">
+        <v>282</v>
+      </c>
+      <c r="E31" s="28" t="s">
+        <v>283</v>
+      </c>
+      <c r="F31" s="16" t="s">
         <v>194</v>
       </c>
-      <c r="G31" s="24" t="s">
+      <c r="G31" s="16" t="s">
         <v>257</v>
       </c>
-      <c r="H31" s="36" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" ht="12">
+      <c r="H31" s="43" t="s">
+        <v>270</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="36">
       <c r="A32" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="26" t="s">
         <v>162</v>
       </c>
-      <c r="C32" s="19" t="s">
+      <c r="C32" s="27" t="s">
         <v>187</v>
       </c>
-      <c r="D32" s="20" t="s">
-        <v>208</v>
-      </c>
-      <c r="E32" s="20"/>
-      <c r="F32" s="43" t="s">
+      <c r="D32" s="28" t="s">
+        <v>284</v>
+      </c>
+      <c r="E32" s="28" t="s">
+        <v>285</v>
+      </c>
+      <c r="F32" s="44" t="s">
         <v>198</v>
       </c>
-      <c r="G32" s="24" t="s">
+      <c r="G32" s="16" t="s">
         <v>258</v>
       </c>
-      <c r="H32" s="42"/>
+      <c r="H32" s="35"/>
+      <c r="I32" s="3" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="33" spans="1:8" ht="12">
       <c r="A33" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="29" t="s">
         <v>163</v>
       </c>
-      <c r="C33" s="30" t="s">
+      <c r="C33" s="29" t="s">
         <v>188</v>
       </c>
-      <c r="D33" s="31" t="s">
+      <c r="D33" s="30" t="s">
         <v>227</v>
       </c>
-      <c r="E33" s="31" t="s">
+      <c r="E33" s="30" t="s">
         <v>247</v>
       </c>
-      <c r="F33" s="32" t="s">
+      <c r="F33" s="31" t="s">
         <v>190</v>
       </c>
-      <c r="G33" s="32"/>
-      <c r="H33" s="37"/>
+      <c r="G33" s="31"/>
+      <c r="H33" s="35"/>
     </row>
     <row r="35" spans="1:8">
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
+      <c r="F35" s="25"/>
+      <c r="G35" s="25"/>
+      <c r="H35" s="25"/>
     </row>
   </sheetData>
   <phoneticPr fontId="7" type="noConversion"/>
@@ -2843,7 +2909,7 @@
   <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15"/>

</xml_diff>